<commit_message>
#2651 - Checklist da Qualidade p/ Gerência (Construção 4)
- Checklist da qualidade das equipes de gerência (GPR, MED, GCO);

- Mesclagem da planilha de GCO que estava separada, em uma planilha com
todos os checklists (Mudança da versão 1.1.0 p/ 1.1.1 por conta dessa
mudança na planilha de GCO).
</commit_message>
<xml_diff>
--- a/Doc-DD-UFG/Qualidade/Gerência/checklist_de_qualidade_de_processo_e_produto_GPR_MED_GCO_1.1.1_SDD-UFG_201512010800.xlsx
+++ b/Doc-DD-UFG/Qualidade/Gerência/checklist_de_qualidade_de_processo_e_produto_GPR_MED_GCO_1.1.1_SDD-UFG_201512010800.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marla Aragão\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marla Aragão\Documents\GitHub\sdd-ufg\Doc-DD-UFG\Qualidade\Gerência\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="81">
   <si>
     <t>Instruções de preenchimento do checklist</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>Não há prazo para auditoria especificado no Plano de Projeto, impossibilitando determinar se já deveria ter ocorrido auditoria ou não para a baseline criada. A auditoria não é de responsabilidade da equipe de GCO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1759,7 +1762,7 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2795,7 +2798,9 @@
       <c r="C29" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="23"/>
+      <c r="D29" s="23" t="s">
+        <v>80</v>
+      </c>
       <c r="E29" s="39" t="s">
         <v>29</v>
       </c>

</xml_diff>